<commit_message>
Update template for line item export
</commit_message>
<xml_diff>
--- a/export/IHR Costing Tool - Line Item Export.xlsx
+++ b/export/IHR Costing Tool - Line Item Export.xlsx
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="35">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="33">
   <si>
     <t>Line item ID</t>
   </si>
@@ -87,54 +87,6 @@
     <t>Staff multiplier unit</t>
   </si>
   <si>
-    <r>
-      <t xml:space="preserve">Do not edit: Base cost amount
-</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="14"/>
-        <color rgb="FFFFFFFF"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>(default value)</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">Do not edit: Quantity
-</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="14"/>
-        <color rgb="FFFFFFFF"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>(product of all multipliers)</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">Do not edit: Total first-year costs
-</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="14"/>
-        <color rgb="FFFFFFFF"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>(product of base cost and quantity)</t>
-    </r>
-  </si>
-  <si>
     <t>P.1.1.1.1.1</t>
   </si>
   <si>
@@ -168,14 +120,17 @@
     <t>days</t>
   </si>
   <si>
-    <t>TBD</t>
+    <t>Do not edit: Recurring costs (annual)</t>
+  </si>
+  <si>
+    <t>Do not edit: Start-up/Capital costs</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -185,13 +140,6 @@
     </font>
     <font>
       <b/>
-      <sz val="14"/>
-      <color rgb="FFFFFFFF"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <sz val="14"/>
       <color rgb="FFFFFFFF"/>
       <name val="Calibri"/>
@@ -284,16 +232,16 @@
     <xf numFmtId="0" fontId="1" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
-    <xf numFmtId="4" fontId="3" fillId="5" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="4" fontId="2" fillId="5" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -616,21 +564,24 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DB0BAA1C-8812-4BC1-86BB-AD3EF649F296}">
-  <dimension ref="A1:W2"/>
+  <dimension ref="A1:V2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C2" sqref="C2"/>
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="15.42578125" customWidth="1"/>
-    <col min="2" max="2" width="46.28515625" customWidth="1"/>
-    <col min="3" max="20" width="25.7109375" customWidth="1"/>
-    <col min="21" max="23" width="50.7109375" customWidth="1"/>
+    <col min="2" max="2" width="51.140625" customWidth="1"/>
+    <col min="3" max="8" width="25.7109375" customWidth="1"/>
+    <col min="9" max="9" width="49.5703125" customWidth="1"/>
+    <col min="10" max="20" width="25.7109375" customWidth="1"/>
+    <col min="21" max="22" width="50.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:23" ht="38.25" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:22" ht="38.25" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -692,21 +643,18 @@
         <v>19</v>
       </c>
       <c r="U1" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="V1" s="3" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="2" spans="1:22" ht="60.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A2" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="V1" s="3" t="s">
+      <c r="B2" s="5" t="s">
         <v>21</v>
-      </c>
-      <c r="W1" s="3" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="2" spans="1:23" ht="90.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="4" t="s">
-        <v>23</v>
-      </c>
-      <c r="B2" s="5" t="s">
-        <v>24</v>
       </c>
       <c r="C2" s="4">
         <v>1</v>
@@ -715,41 +663,41 @@
         <v>2</v>
       </c>
       <c r="E2" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="F2" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="G2" s="6" t="s">
+        <v>24</v>
+      </c>
+      <c r="H2" s="6" t="s">
         <v>25</v>
       </c>
-      <c r="F2" s="4" t="s">
+      <c r="I2" s="6" t="s">
         <v>26</v>
       </c>
-      <c r="G2" s="6" t="s">
+      <c r="J2" s="6" t="s">
         <v>27</v>
-      </c>
-      <c r="H2" s="6" t="s">
-        <v>28</v>
-      </c>
-      <c r="I2" s="6" t="s">
-        <v>29</v>
-      </c>
-      <c r="J2" s="6" t="s">
-        <v>30</v>
       </c>
       <c r="K2" s="7">
         <v>1000</v>
       </c>
       <c r="L2" s="8" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
       <c r="M2" s="6">
         <v>1</v>
       </c>
       <c r="N2" s="6" t="s">
-        <v>32</v>
+        <v>29</v>
       </c>
       <c r="O2" s="6">
         <f>60*Q2</f>
         <v>60</v>
       </c>
       <c r="P2" s="6" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
       <c r="Q2" s="6">
         <v>1</v>
@@ -758,17 +706,17 @@
       <c r="S2" s="6"/>
       <c r="T2" s="6"/>
       <c r="U2" s="9">
-        <v>20</v>
-      </c>
-      <c r="V2" s="8" t="s">
-        <v>34</v>
-      </c>
-      <c r="W2" s="8" t="s">
-        <v>34</v>
+        <f>IF(OR($H2="Start-up",$H2="Capital"),1,0)*IF($M2="",1,$M2)*IF($O2="",1,$O2)*IF($Q2="",1,$Q2)*IF($S2="",1,$S2)*IF($K2="",1,$K2)</f>
+        <v>60000</v>
+      </c>
+      <c r="V2" s="9">
+        <f>IF(OR($H2="Start-up",$H2="Capital"),0,1)*IF($M2="",1,$M2)*IF($O2="",1,$O2)*IF($Q2="",1,$Q2)*IF($S2="",1,$S2)*IF($K2="",1,$K2)</f>
+        <v>0</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 

</xml_diff>

<commit_message>
Add error proofing to line item templat
</commit_message>
<xml_diff>
--- a/export/IHR Costing Tool - Line Item Export.xlsx
+++ b/export/IHR Costing Tool - Line Item Export.xlsx
@@ -566,9 +566,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DB0BAA1C-8812-4BC1-86BB-AD3EF649F296}">
   <dimension ref="A1:V2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="M1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
+      <selection pane="bottomLeft" activeCell="O2" sqref="O2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -693,7 +693,6 @@
         <v>29</v>
       </c>
       <c r="O2" s="6">
-        <f>60*Q2</f>
         <v>60</v>
       </c>
       <c r="P2" s="6" t="s">
@@ -706,11 +705,11 @@
       <c r="S2" s="6"/>
       <c r="T2" s="6"/>
       <c r="U2" s="9">
-        <f>IF(OR($H2="Start-up",$H2="Capital"),1,0)*IF($M2="",1,$M2)*IF($O2="",1,$O2)*IF($Q2="",1,$Q2)*IF($S2="",1,$S2)*IF($K2="",1,$K2)</f>
+        <f>IFERROR(IF(OR($H2="Start-up",$H2="Capital"),1,0)*IF($M2="",1,$M2)*IF($O2="",1,$O2)*IF($Q2="",1,$Q2)*IF($S2="",1,$S2)*IF($K2="",1,$K2),"")</f>
         <v>60000</v>
       </c>
       <c r="V2" s="9">
-        <f>IF(OR($H2="Start-up",$H2="Capital"),0,1)*IF($M2="",1,$M2)*IF($O2="",1,$O2)*IF($Q2="",1,$Q2)*IF($S2="",1,$S2)*IF($K2="",1,$K2)</f>
+        <f>IFERROR(IF(OR($H2="Start-up",$H2="Capital"),0,1)*IF($M2="",1,$M2)*IF($O2="",1,$O2)*IF($Q2="",1,$Q2)*IF($S2="",1,$S2)*IF($K2="",1,$K2),"")</f>
         <v>0</v>
       </c>
     </row>

</xml_diff>

<commit_message>
rmv example from template
</commit_message>
<xml_diff>
--- a/export/IHR Costing Tool - Line Item Export.xlsx
+++ b/export/IHR Costing Tool - Line Item Export.xlsx
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="33">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="22">
   <si>
     <t>Line item ID</t>
   </si>
@@ -85,39 +85,6 @@
   </si>
   <si>
     <t>Staff multiplier unit</t>
-  </si>
-  <si>
-    <t>P.1.1.1.1.1</t>
-  </si>
-  <si>
-    <t>P.1.1 Legislation, laws, regulations, administrative requirements, policies or other government instruments in place are sufficient for implementation of IHR.</t>
-  </si>
-  <si>
-    <t>Review and revise IHR legislation</t>
-  </si>
-  <si>
-    <t>Hire national consultant to provide expert advice</t>
-  </si>
-  <si>
-    <t>Daily fees (total)</t>
-  </si>
-  <si>
-    <t>Start-up</t>
-  </si>
-  <si>
-    <t>Fees for 60-days of consultant time to provide expert advice regarding the development of legislation and regulation for IHR implementation</t>
-  </si>
-  <si>
-    <t>Consultant fees (daily)</t>
-  </si>
-  <si>
-    <t>per day</t>
-  </si>
-  <si>
-    <t>Central area count</t>
-  </si>
-  <si>
-    <t>days</t>
   </si>
   <si>
     <t>Do not edit: Recurring costs (annual)</t>
@@ -566,9 +533,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DB0BAA1C-8812-4BC1-86BB-AD3EF649F296}">
   <dimension ref="A1:V2"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="M1" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="J1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="O2" sqref="O2"/>
+      <selection pane="bottomLeft" activeCell="S1" sqref="S1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -643,74 +610,40 @@
         <v>19</v>
       </c>
       <c r="U1" s="3" t="s">
-        <v>32</v>
+        <v>21</v>
       </c>
       <c r="V1" s="3" t="s">
-        <v>31</v>
+        <v>20</v>
       </c>
     </row>
-    <row r="2" spans="1:22" ht="60.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="4" t="s">
-        <v>20</v>
-      </c>
-      <c r="B2" s="5" t="s">
-        <v>21</v>
-      </c>
-      <c r="C2" s="4">
-        <v>1</v>
-      </c>
-      <c r="D2" s="4">
-        <v>2</v>
-      </c>
-      <c r="E2" s="4" t="s">
-        <v>22</v>
-      </c>
-      <c r="F2" s="4" t="s">
-        <v>23</v>
-      </c>
-      <c r="G2" s="6" t="s">
-        <v>24</v>
-      </c>
-      <c r="H2" s="6" t="s">
-        <v>25</v>
-      </c>
-      <c r="I2" s="6" t="s">
-        <v>26</v>
-      </c>
-      <c r="J2" s="6" t="s">
-        <v>27</v>
-      </c>
-      <c r="K2" s="7">
-        <v>1000</v>
-      </c>
-      <c r="L2" s="8" t="s">
-        <v>28</v>
-      </c>
-      <c r="M2" s="6">
-        <v>1</v>
-      </c>
-      <c r="N2" s="6" t="s">
-        <v>29</v>
-      </c>
-      <c r="O2" s="6">
-        <v>60</v>
-      </c>
-      <c r="P2" s="6" t="s">
-        <v>30</v>
-      </c>
-      <c r="Q2" s="6">
-        <v>1</v>
-      </c>
+    <row r="2" spans="1:22" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A2" s="4"/>
+      <c r="B2" s="5"/>
+      <c r="C2" s="4"/>
+      <c r="D2" s="4"/>
+      <c r="E2" s="4"/>
+      <c r="F2" s="4"/>
+      <c r="G2" s="6"/>
+      <c r="H2" s="6"/>
+      <c r="I2" s="6"/>
+      <c r="J2" s="6"/>
+      <c r="K2" s="7"/>
+      <c r="L2" s="8"/>
+      <c r="M2" s="6"/>
+      <c r="N2" s="6"/>
+      <c r="O2" s="6"/>
+      <c r="P2" s="6"/>
+      <c r="Q2" s="6"/>
       <c r="R2" s="6"/>
       <c r="S2" s="6"/>
       <c r="T2" s="6"/>
       <c r="U2" s="9">
         <f>IFERROR(IF(OR($H2="Start-up",$H2="Capital"),1,0)*IF($M2="",1,$M2)*IF($O2="",1,$O2)*IF($Q2="",1,$Q2)*IF($S2="",1,$S2)*IF($K2="",1,$K2),"")</f>
-        <v>60000</v>
+        <v>0</v>
       </c>
       <c r="V2" s="9">
         <f>IFERROR(IF(OR($H2="Start-up",$H2="Capital"),0,1)*IF($M2="",1,$M2)*IF($O2="",1,$O2)*IF($Q2="",1,$Q2)*IF($S2="",1,$S2)*IF($K2="",1,$K2),"")</f>
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Tweaks to export templates
</commit_message>
<xml_diff>
--- a/export/IHR Costing Tool - Line Item Export.xlsx
+++ b/export/IHR Costing Tool - Line Item Export.xlsx
@@ -533,9 +533,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DB0BAA1C-8812-4BC1-86BB-AD3EF649F296}">
   <dimension ref="A1:V1500"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="L1" sqref="L1"/>
+      <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
Updated line item export template
</commit_message>
<xml_diff>
--- a/export/IHR Costing Tool - Line Item Export.xlsx
+++ b/export/IHR Costing Tool - Line Item Export.xlsx
@@ -13,7 +13,7 @@
   </bookViews>
   <sheets>
     <sheet name="Costs" sheetId="1" r:id="rId1"/>
-    <sheet name="Instructions" sheetId="2" r:id="rId2"/>
+    <sheet name="Legend" sheetId="3" r:id="rId2"/>
   </sheets>
   <calcPr calcId="171027"/>
   <extLst>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="22">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="107" uniqueCount="72">
   <si>
     <t>Line item ID</t>
   </si>
@@ -92,12 +92,333 @@
   <si>
     <t>Do not edit: Annual recurring costs</t>
   </si>
+  <si>
+    <t>Column name</t>
+  </si>
+  <si>
+    <t>Definition</t>
+  </si>
+  <si>
+    <t>Example</t>
+  </si>
+  <si>
+    <t>Valid column values</t>
+  </si>
+  <si>
+    <t>An indicator JEE ID (e.g., P.1.1) follow by its name</t>
+  </si>
+  <si>
+    <t>Unique ID and name of the indicator costed</t>
+  </si>
+  <si>
+    <t>User's starting score for the indicator</t>
+  </si>
+  <si>
+    <t>1, 2, 3, 4, or 5</t>
+  </si>
+  <si>
+    <t>User's target score for the indicator</t>
+  </si>
+  <si>
+    <t>2, 3, 4, or 5</t>
+  </si>
+  <si>
+    <t>D.1.1 Laboratory testing for detection of priority diseases</t>
+  </si>
+  <si>
+    <t>Implement and review national IHR laboratory plan</t>
+  </si>
+  <si>
+    <t>Hold annual national conference on IHR laboratory plan implementation and coordination</t>
+  </si>
+  <si>
+    <t>Conference per diems</t>
+  </si>
+  <si>
+    <t>Recurring</t>
+  </si>
+  <si>
+    <t>Per diems for annual, medium, 3-day, national conference on national IHR laboratory plan</t>
+  </si>
+  <si>
+    <t>D.1.1.4.1.2</t>
+  </si>
+  <si>
+    <t>Per diem for meeting - Domestic</t>
+  </si>
+  <si>
+    <t>per day</t>
+  </si>
+  <si>
+    <t>Central area count</t>
+  </si>
+  <si>
+    <t>1</t>
+  </si>
+  <si>
+    <t>annual conference</t>
+  </si>
+  <si>
+    <t>3</t>
+  </si>
+  <si>
+    <t>days</t>
+  </si>
+  <si>
+    <t>Meeting attendees - Medium</t>
+  </si>
+  <si>
+    <t>Name of the action costed for the indicator</t>
+  </si>
+  <si>
+    <t>Name of the input costed for the action</t>
+  </si>
+  <si>
+    <t>Name of the line item costed for the input</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">Start-up: </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">Line item amount repesents professional services, workshops, or similar only paid in budget year 1 (e.g., consultant fees)
+</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Capital</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">: Line item amount represents durable goods, physical infrastructure, or similar only paid in budget year 1 (e.g., desktop computer)
+</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Recurring:</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> Line item amount paid once in every budget year including budget year 1 (e.g., salaries)</t>
+    </r>
+  </si>
+  <si>
+    <t>Description of the line item costed for the input</t>
+  </si>
+  <si>
+    <t>Unique ID of the line item costed for the input</t>
+  </si>
+  <si>
+    <t>The name of the base cost of the line item (e.g., the amount paid for one desktop computer)</t>
+  </si>
+  <si>
+    <t>The unit of the base cost</t>
+  </si>
+  <si>
+    <t>The base cost of the line item. Adjusting this value for a line item will update the total amount calculated in the final two columns.</t>
+  </si>
+  <si>
+    <t>The value of the country multiplier (see column O). Adjusting this value for a line item will update the total amount calculated in the final two columns.</t>
+  </si>
+  <si>
+    <t>The country multiplier used to scale the base cost of this line item (e.g., the number of intermediate areas in the country)</t>
+  </si>
+  <si>
+    <t>The value of custom multiplier 1 (see column Q). Adjusting this value for a line item will update the total amount calculated in the final two columns.</t>
+  </si>
+  <si>
+    <t>The first custom multiplier used to scale the base  cost of this line item</t>
+  </si>
+  <si>
+    <t>The value of custom multiplier 2 (see column S). Adjusting this value for a line item will update the total amount calculated in the final two columns.</t>
+  </si>
+  <si>
+    <t>The second custom multiplier used to scale the base  cost of this line item</t>
+  </si>
+  <si>
+    <t>The value of the staff multiplier (see column U). Adjusting this value for a line item will update the total amount calculated in the final two columns.</t>
+  </si>
+  <si>
+    <t>The staff multiplier used to scale the base cost of this line item (e.g., the number of attendees for a medium meeting)</t>
+  </si>
+  <si>
+    <t>Start-up/Capital costs</t>
+  </si>
+  <si>
+    <t>Annual recurring costs</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">For inputs (gray rows): </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">The total start-up/capital costs for the input. If the user entered a custom value for the input's costs in the IHR Costing Tool, that value is shown. Otherwise, the default value of the input's cost is shown.  Note: Editing the costs of an input's line items (white rows) will not automatically update the input's total costs
+</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>For line items (white rows):</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> The total start-up/capital costs for the line item, if it is labeled "Start-up" or "Capital" in column G</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">For inputs (gray rows): </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">The total annual recurring costs for the input. If the user entered a custom value for the input's costs in the IHR Costing Tool, that value is shown. Otherwise, the default value of the input's cost is shown.  Note: Editing the costs of an input's line items (white rows) will not automatically update the input's total costs
+</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>For line items (white rows):</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> The total annual recurring costs for the line item, if it is labeled "Recurring" in column G</t>
+    </r>
+  </si>
+  <si>
+    <t>Any non-zero number</t>
+  </si>
+  <si>
+    <t>Any line item ID</t>
+  </si>
+  <si>
+    <t>Any text without line breaks</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <u/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">One of the following:
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Start-up
+Capital
+Recurring</t>
+    </r>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -128,8 +449,31 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="14"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="6">
+  <fills count="7">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -160,6 +504,12 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.59999389629810485"/>
+        <bgColor theme="4"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="2">
     <border>
@@ -188,7 +538,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="22">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
@@ -216,6 +566,42 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="4" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="4" fontId="0" fillId="5" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="4" fontId="0" fillId="5" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -36599,13 +36985,309 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7B383B50-BA14-4F54-A0AF-B9C5E7C62A21}">
-  <dimension ref="A1"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0B62A33A-A79D-4D31-A8E3-5D09AAE70E3B}">
+  <dimension ref="A1:W4"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <pane xSplit="1" topLeftCell="B1" activePane="topRight" state="frozen"/>
+      <selection pane="topRight"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData/>
+  <cols>
+    <col min="1" max="1" width="24" style="11" customWidth="1"/>
+    <col min="2" max="7" width="38.7109375" style="11" customWidth="1"/>
+    <col min="8" max="8" width="50.7109375" style="11" customWidth="1"/>
+    <col min="9" max="21" width="38.7109375" style="11" customWidth="1"/>
+    <col min="22" max="23" width="50.7109375" style="11" customWidth="1"/>
+    <col min="24" max="16384" width="9.140625" style="11"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:23" ht="38.25" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A1" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="I1" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="J1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="K1" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="L1" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="M1" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="N1" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="O1" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="P1" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="Q1" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="R1" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="S1" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="T1" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="U1" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="V1" s="3" t="s">
+        <v>64</v>
+      </c>
+      <c r="W1" s="3" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="2" spans="1:23" s="20" customFormat="1" ht="180" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A2" s="10" t="s">
+        <v>23</v>
+      </c>
+      <c r="B2" s="12" t="s">
+        <v>27</v>
+      </c>
+      <c r="C2" s="12" t="s">
+        <v>28</v>
+      </c>
+      <c r="D2" s="12" t="s">
+        <v>30</v>
+      </c>
+      <c r="E2" s="12" t="s">
+        <v>47</v>
+      </c>
+      <c r="F2" s="12" t="s">
+        <v>48</v>
+      </c>
+      <c r="G2" s="17" t="s">
+        <v>49</v>
+      </c>
+      <c r="H2" s="17" t="s">
+        <v>50</v>
+      </c>
+      <c r="I2" s="17" t="s">
+        <v>51</v>
+      </c>
+      <c r="J2" s="17" t="s">
+        <v>52</v>
+      </c>
+      <c r="K2" s="17" t="s">
+        <v>53</v>
+      </c>
+      <c r="L2" s="17" t="s">
+        <v>55</v>
+      </c>
+      <c r="M2" s="17" t="s">
+        <v>54</v>
+      </c>
+      <c r="N2" s="17" t="s">
+        <v>56</v>
+      </c>
+      <c r="O2" s="17" t="s">
+        <v>57</v>
+      </c>
+      <c r="P2" s="17" t="s">
+        <v>58</v>
+      </c>
+      <c r="Q2" s="17" t="s">
+        <v>59</v>
+      </c>
+      <c r="R2" s="17" t="s">
+        <v>60</v>
+      </c>
+      <c r="S2" s="17" t="s">
+        <v>61</v>
+      </c>
+      <c r="T2" s="17" t="s">
+        <v>62</v>
+      </c>
+      <c r="U2" s="17" t="s">
+        <v>63</v>
+      </c>
+      <c r="V2" s="19" t="s">
+        <v>66</v>
+      </c>
+      <c r="W2" s="19" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="3" spans="1:23" s="16" customFormat="1" ht="75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A3" s="10" t="s">
+        <v>25</v>
+      </c>
+      <c r="B3" s="12" t="s">
+        <v>26</v>
+      </c>
+      <c r="C3" s="12" t="s">
+        <v>29</v>
+      </c>
+      <c r="D3" s="12" t="s">
+        <v>31</v>
+      </c>
+      <c r="E3" s="13" t="s">
+        <v>70</v>
+      </c>
+      <c r="F3" s="13" t="s">
+        <v>70</v>
+      </c>
+      <c r="G3" s="13" t="s">
+        <v>70</v>
+      </c>
+      <c r="H3" s="13" t="s">
+        <v>71</v>
+      </c>
+      <c r="I3" s="13" t="s">
+        <v>70</v>
+      </c>
+      <c r="J3" s="13" t="s">
+        <v>69</v>
+      </c>
+      <c r="K3" s="13" t="s">
+        <v>70</v>
+      </c>
+      <c r="L3" s="13" t="s">
+        <v>68</v>
+      </c>
+      <c r="M3" s="13" t="s">
+        <v>70</v>
+      </c>
+      <c r="N3" s="13" t="s">
+        <v>68</v>
+      </c>
+      <c r="O3" s="13" t="s">
+        <v>70</v>
+      </c>
+      <c r="P3" s="13" t="s">
+        <v>68</v>
+      </c>
+      <c r="Q3" s="13" t="s">
+        <v>70</v>
+      </c>
+      <c r="R3" s="13" t="s">
+        <v>68</v>
+      </c>
+      <c r="S3" s="13" t="s">
+        <v>70</v>
+      </c>
+      <c r="T3" s="13" t="s">
+        <v>68</v>
+      </c>
+      <c r="U3" s="13" t="s">
+        <v>70</v>
+      </c>
+      <c r="V3" s="15" t="s">
+        <v>68</v>
+      </c>
+      <c r="W3" s="15" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="4" spans="1:23" s="20" customFormat="1" ht="75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A4" s="10" t="s">
+        <v>24</v>
+      </c>
+      <c r="B4" s="21" t="s">
+        <v>32</v>
+      </c>
+      <c r="C4" s="12">
+        <v>1</v>
+      </c>
+      <c r="D4" s="12">
+        <v>2</v>
+      </c>
+      <c r="E4" s="12" t="s">
+        <v>33</v>
+      </c>
+      <c r="F4" s="12" t="s">
+        <v>34</v>
+      </c>
+      <c r="G4" s="17" t="s">
+        <v>35</v>
+      </c>
+      <c r="H4" s="17" t="s">
+        <v>36</v>
+      </c>
+      <c r="I4" s="17" t="s">
+        <v>37</v>
+      </c>
+      <c r="J4" s="17" t="s">
+        <v>38</v>
+      </c>
+      <c r="K4" s="17" t="s">
+        <v>39</v>
+      </c>
+      <c r="L4" s="14">
+        <v>105</v>
+      </c>
+      <c r="M4" s="18" t="s">
+        <v>40</v>
+      </c>
+      <c r="N4" s="17">
+        <v>1</v>
+      </c>
+      <c r="O4" s="17" t="s">
+        <v>41</v>
+      </c>
+      <c r="P4" s="17" t="s">
+        <v>42</v>
+      </c>
+      <c r="Q4" s="17" t="s">
+        <v>43</v>
+      </c>
+      <c r="R4" s="17" t="s">
+        <v>44</v>
+      </c>
+      <c r="S4" s="17" t="s">
+        <v>45</v>
+      </c>
+      <c r="T4" s="17">
+        <v>30</v>
+      </c>
+      <c r="U4" s="17" t="s">
+        <v>46</v>
+      </c>
+      <c r="V4" s="19">
+        <v>0</v>
+      </c>
+      <c r="W4" s="19">
+        <v>9450</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>

</xml_diff>